<commit_message>
0402 4thViewPage AlmostFinished Commit
</commit_message>
<xml_diff>
--- a/프로젝트 기획서_콜미백.xlsx
+++ b/프로젝트 기획서_콜미백.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="438">
   <si>
     <t>프로젝트 기획서</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2407,6 +2407,70 @@
   </si>
   <si>
     <t xml:space="preserve">프로젝트 이름, 프로젝트 내용, 등록일, 마감일, 구분, 제작자, 최근 업데이트, 업데이트 내역(업데이트한 사람, 업데이트 시간, 업데이트 내용) 상태 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 업데이트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21SS 룩북</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진-인물-화보-의류 및 잡화-의류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셀프 프로젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남재민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남재민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행중</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2828,7 +2892,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3026,6 +3090,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4684,8 +4754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H28" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5585,27 +5655,27 @@
         <v>421</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="20" t="s">
+    <row r="41" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="F41" s="28" t="s">
+      <c r="F41" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="G41" s="28"/>
-      <c r="H41" s="24" t="s">
+      <c r="G41" s="46"/>
+      <c r="H41" s="45" t="s">
         <v>355</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I41" s="47" t="s">
         <v>382</v>
       </c>
     </row>
@@ -5631,27 +5701,27 @@
       </c>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="20" t="s">
+    <row r="43" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D43" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="45" t="s">
         <v>360</v>
       </c>
-      <c r="F43" s="28" t="s">
+      <c r="F43" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="28"/>
-      <c r="H43" s="24" t="s">
+      <c r="G43" s="46"/>
+      <c r="H43" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" s="47" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6253,17 +6323,91 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C13:F17"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="66" customWidth="1"/>
+    <col min="4" max="4" width="32" style="66" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="66" customWidth="1"/>
+    <col min="6" max="6" width="32" style="66" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="66" t="s">
+        <v>422</v>
+      </c>
+      <c r="D13" s="66">
+        <v>1</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>429</v>
+      </c>
+      <c r="F13" s="66" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="66" t="s">
+        <v>423</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>432</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>427</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="66" t="s">
+        <v>424</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>433</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>428</v>
+      </c>
+      <c r="F15" s="66" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="66" t="s">
+        <v>425</v>
+      </c>
+      <c r="D16" s="67">
+        <v>44280</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>430</v>
+      </c>
+      <c r="F16" s="66" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="66" t="s">
+        <v>426</v>
+      </c>
+      <c r="D17" s="67">
+        <v>44297</v>
+      </c>
+      <c r="E17" s="66" t="s">
+        <v>431</v>
+      </c>
+      <c r="F17" s="67">
+        <v>44286</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
0406 ViewPage 90% Commit
</commit_message>
<xml_diff>
--- a/프로젝트 기획서_콜미백.xlsx
+++ b/프로젝트 기획서_콜미백.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17685" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="446">
   <si>
     <t>프로젝트 기획서</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,10 +205,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>사진 - 인물 - 화보 - 컨셉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사진 - 인물 - 착장 - 제품 디테일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,14 +289,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(마우스오버) 착장의 디테일을 볼 수 있는 사진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(마우스오버) 의류 및 패션 잡화류</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>(마우스오버) 완성된 메이크업을 받은 모델</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -311,10 +307,129 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">중점이 되는 것은 무엇인가요? </t>
-    </r>
-    <r>
-      <rPr>
+      <t>품목을 선택해주세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - (마우스오버) 모든 의류</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 인테리어 및 각종 소품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 가방, 모자 등 유리, 금속이 아닌 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 모든 신발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 시계, 쥬얼리 등 유리, 금속으로 이루어진 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버)착용한 제품 위주의 인물컷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업 - 제품 화보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - 뷰티&amp;메이크업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - 의류 및 잡화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - 인테리어 및 소품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업 - 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 의류 및 잡화 - 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 착장 - 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - 식료품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - 가전 및 전자제품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - (공통)제품 누끼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - (공통)컨셉 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 제품 - (공통)모델 착용 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 착장 - 누끼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 모든 의류 제품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 조명, 장식품, 가구 및 각종 실내 소품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 가전 및 전자제품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 포장 식품, 조리한 음식, 식자재, 음료 및 주류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="맑은 고딕"/>
@@ -322,12 +437,39 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- (마우스오버) 메이크업 제품</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 완성된 메이크업을 받은 모델</t>
+      <t xml:space="preserve">어떻게 찍고 싶으신가요? - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(마우스오버) 심플한 배경의 제품 사진</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 소품 및 배경을 활용한 제품 컨셉 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 모델 착용 및 사용 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 건물 전경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 실내 구조 및 인테리어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 대형 조각품 및 예술품 등 구조물</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -341,137 +483,10 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>품목을 선택해주세요</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - (마우스오버) 모든 의류</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 소품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 인테리어 및 각종 소품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 가방, 모자 등 유리, 금속이 아닌 것</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 모든 신발</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 시계, 쥬얼리 등 유리, 금속으로 이루어진 것</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버)착용한 제품 위주의 인물컷</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업 - 제품 화보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업 - 메이크업 화보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - 뷰티&amp;메이크업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - 의류 및 잡화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - 인테리어 및 소품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업 - 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 화보 - 의류 및 잡화 - 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 착장 - 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - 식료품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - 가전 및 전자제품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - 기타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - (공통)제품 누끼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - (공통)컨셉 사진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 제품 - (공통)모델 착용 사진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진 - 인물 - 착장 - 누끼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 모든 의류 제품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 조명, 장식품, 가구 및 각종 실내 소품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 가전 및 전자제품</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 포장 식품, 조리한 음식, 식자재, 음료 및 주류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">어디에 쓰일 사진일까요? </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="맑은 고딕"/>
@@ -479,73 +494,8 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">어떻게 찍고 싶으신가요? - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(마우스오버) 심플한 배경의 제품 사진</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 소품 및 배경을 활용한 제품 컨셉 사진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 모델 착용 및 사용 사진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 건물 전경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 실내 구조 및 인테리어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 대형 조각품 및 예술품 등 구조물</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">어디에 쓰일 사진일까요? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>- (마우스오버) 인쇄 및 웹 배포 등 다용도로 사용될 사진</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 현수막, 대형 포스터 등 대화면 인쇄용 고화질 사진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(마우스오버) 팜플렛, 책자 등 일반 인쇄용 고화질 사진</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -644,32 +594,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>어떤 것을 사진에 담으실 건가요?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - (마우스오버) 모델 메이크업 또는 메이크업 제품</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(마우스오버) 예술 및 컨셉 사진</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1444,10 +1368,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>addProject.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>projects.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1682,18 +1602,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>project.addProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>img.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/addProject/select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/addProject/img</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1946,531 +1858,766 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>beauty.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/clothes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.beauty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.clothes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뷰티 사진 종류 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의류 및 잡화 종류 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beautyP, clothesP, goodsP, electro, food, etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/beautyP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/clothesP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/goodsP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/electro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>food.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/food</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.food</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식료품 사진 종류 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>productPic.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>productPic.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뷰티 제품 사진 종류 선택(공통)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의류 및 잡화 제품 사진 종류 선택(공통)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소품 사진 종류 선택(공통)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가전제품 사진 종류 선택(공통)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.productPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.productPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.productPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>picSize.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/picSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.picSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 사이즈 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projectDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>picSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>picSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>picSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addProjectFin.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 추가 완료 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projects, main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(login, signup, )addProjectPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>askLogin.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.addProjectPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.askLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 할지 확인하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 정보 최종 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 추가 완료 페이지 (프로젝트 목록, 메인페이지로 이동)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editProjectPro, projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delProjectPro.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/delProjectPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.delProjectPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 삭제 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delProjectPro, projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>review.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/askLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 로그인 유무에 따라 로그인할지 말지 표시 / 비로그인으로 진행할 경우 등록날짜,시간,번호 조합해서 ID 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projectInfo, editProject, delProject, login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원 프로젝트 조회를 위한 로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원으로 등록한 프로젝트를 조회할 때 발급받은 ID 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editProject, delProject, projects, addComment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코멘트 입력 창 생성 / 체크박스 / 라디오 박스로 시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projects, addCommentPro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 추가 시 마지막에 projectDetail 창에서 입력한 정보만 수정할 수 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인 회원 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/editPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.editPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editPasswordPro, profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editPassword, projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 검사 해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newProject.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새 프로젝트 추가 안내</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logout.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 &amp; 비밀번호 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원(이름, 아이디, 비밀번호, 가입일자, 생성 프로젝트 갯수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updateProfilePro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/updateProfilePro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.updateProfilePro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인정보 변경 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchLoginInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/searchLoginInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.searchLoginInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셀프 프로젝트 / 의뢰받은 프로젝트 / 의뢰한 프로젝트 / 완료된 프로젝트 - 비로그인일 경우 로그인 화면으로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력/처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB비교해서 정보 바로 alert로 띄우기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">프로젝트 이름, 프로젝트 내용, 등록일, 마감일, 구분, 제작자, 최근 업데이트, 업데이트 내역(업데이트한 사람, 업데이트 시간, 업데이트 내용) 상태 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 업데이트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21SS 룩북</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진-인물-화보-의류 및 잡화-의류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>셀프 프로젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남재민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남재민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkProjectId.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>signup, login, checkProjectId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/checkProjectId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customer.checkProjectId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/newProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.newProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectProject.jsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addProject/selectProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project.selectProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>어떤</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 촬영을 의뢰</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>하고</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 싶으</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>신가요?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - (마우스오버) 인물</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 건물이나 인테리어, 야외 전경, 대형 구조물 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 3D, 기하학, 패턴 등 그래픽 이미지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 착장의 디테일을 볼 수 있는 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 의류 및 잡화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 의류 및 패션 잡화류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 소품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 컨셉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 예술 및 컨셉 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>beauty, clothes, goods, concept, etc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>beauty.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/clothes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.beauty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.clothes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뷰티 사진 종류 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>의류 및 잡화 종류 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>beautyP, clothesP, goodsP, electro, food, etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/beautyP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/clothesP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/goodsP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/electro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>food.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/food</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.food</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>식료품 사진 종류 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>productPic.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>productPic.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뷰티 제품 사진 종류 선택(공통)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>의류 및 잡화 제품 사진 종류 선택(공통)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소품 사진 종류 선택(공통)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가전제품 사진 종류 선택(공통)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.productPic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.productPic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.productPic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>picSize.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/picSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.picSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이미지 사이즈 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projectDetail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>picSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>picSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>picSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/fin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addProjectFin.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.fin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 추가 완료 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projects, main</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(login, signup, )addProjectPro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>askLogin.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.addProjectPro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.askLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 할지 확인하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 정보 최종 검토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 추가 완료 페이지 (프로젝트 목록, 메인페이지로 이동)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editProjectPro, projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delProjectPro.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/delProjectPro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.delProjectPro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 삭제 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delProjectPro, projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>review.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/review</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.review</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/pro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/askLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>현재 로그인 유무에 따라 로그인할지 말지 표시 / 비로그인으로 진행할 경우 등록날짜,시간,번호 조합해서 ID 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projectInfo, editProject, delProject, login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>signup, login, inputId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inputId.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/inputId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.inputId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비회원 프로젝트 조회를 위한 로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비회원으로 등록한 프로젝트를 조회할 때 발급받은 ID 입력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editProject, delProject, projects, addComment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>코멘트 입력 창 생성 / 체크박스 / 라디오 박스로 시간</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projects, addCommentPro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 추가 시 마지막에 projectDetail 창에서 입력한 정보만 수정할 수 있음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/profile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.profile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개인 회원 정보 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/editPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.editPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비밀번호 변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>profile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editPasswordPro, profile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editPassword, projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 검사 해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>newProject.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addProject/new</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project.new</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새 프로젝트 추가 안내</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>logout.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디 &amp; 비밀번호 찾기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원(이름, 아이디, 비밀번호, 가입일자, 생성 프로젝트 갯수)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>profile.jsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>updateProfilePro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/updateProfilePro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.updateProfilePro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개인정보 변경 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchLoginInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/searchLoginInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customer.searchLoginInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>셀프 프로젝트 / 의뢰받은 프로젝트 / 의뢰한 프로젝트 / 완료된 프로젝트 - 비로그인일 경우 로그인 화면으로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출력/처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB비교해서 정보 바로 alert로 띄우기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">프로젝트 이름, 프로젝트 내용, 등록일, 마감일, 구분, 제작자, 최근 업데이트, 업데이트 내역(업데이트한 사람, 업데이트 시간, 업데이트 내용) 상태 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마감일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>등록자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제작자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최근 업데이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>21SS 룩북</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사진-인물-화보-의류 및 잡화-의류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>셀프 프로젝트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>남재민</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>남재민</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>진행중</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>어떤 것을 사진에 담으실 건가요?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - (마우스오버) 모델 메이크업 또는 메이크업 제품</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">중점이 되는 것은 무엇인가요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- (마우스오버) 메이크업 제품</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 - 인물 - 화보 - 뷰티&amp;메이크업 - 메이크업 화보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>품목을 선택해주세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - (마우스오버) 모든 의류</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>안내문구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(공통 : 구분이 모호하다면 왼쪽에 있는 옵션을 선택하세요)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 현수막, 대형 포스터 등 대화면 인쇄용 고화질 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(마우스오버) 팜플렛, 책자 등 일반 인쇄용 고화질 사진</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3037,6 +3184,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3090,12 +3243,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3120,19 +3267,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1828574</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>199821</xdr:rowOff>
+      <xdr:colOff>1933337</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>37880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPr id="3" name="그림 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3145,8 +3292,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1104900" y="7000875"/>
-          <a:ext cx="1809524" cy="1628571"/>
+          <a:off x="1114425" y="6953250"/>
+          <a:ext cx="1904762" cy="1761905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3429,7 +3576,7 @@
   <dimension ref="B1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D23" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3444,12 +3591,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -3494,37 +3641,37 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48" t="s">
-        <v>136</v>
+      <c r="B6" s="50" t="s">
+        <v>128</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>130</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="49"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="49"/>
+        <v>129</v>
+      </c>
+      <c r="D7" s="51"/>
       <c r="E7" s="12" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="55" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="50" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -3532,21 +3679,21 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="54"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="56"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="54"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="59" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -3554,33 +3701,33 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="54"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D11" s="54"/>
+        <v>152</v>
+      </c>
+      <c r="D11" s="56"/>
       <c r="E11" s="6" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="54"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="55"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="12" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3588,21 +3735,21 @@
     </row>
     <row r="15" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3630,7 +3777,7 @@
     <row r="24" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3639,7 +3786,7 @@
     <row r="26" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3728,8 +3875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3748,758 +3895,758 @@
   <sheetData>
     <row r="1" spans="2:9" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
-        <v>90</v>
+      <c r="B2" s="50" t="s">
+        <v>83</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>158</v>
+      <c r="D2" s="63" t="s">
+        <v>443</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>159</v>
+        <v>37</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>151</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>158</v>
+        <v>123</v>
+      </c>
+      <c r="H2" s="66" t="s">
+        <v>150</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="56"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="64"/>
       <c r="E3" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="54"/>
+        <v>429</v>
+      </c>
+      <c r="F3" s="56"/>
       <c r="G3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="65"/>
+        <v>84</v>
+      </c>
+      <c r="H3" s="67"/>
       <c r="I3" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="56"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="54"/>
+        <v>44</v>
+      </c>
+      <c r="F4" s="56"/>
       <c r="G4" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="65"/>
+        <v>85</v>
+      </c>
+      <c r="H4" s="67"/>
       <c r="I4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="56"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="D5" s="62"/>
+        <v>253</v>
+      </c>
+      <c r="D5" s="64"/>
       <c r="E5" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="F5" s="54"/>
+        <v>430</v>
+      </c>
+      <c r="F5" s="56"/>
       <c r="G5" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="H5" s="65"/>
+        <v>255</v>
+      </c>
+      <c r="H5" s="67"/>
       <c r="I5" s="6" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="56"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="64"/>
       <c r="E6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="54"/>
+        <v>431</v>
+      </c>
+      <c r="F6" s="56"/>
       <c r="G6" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="65"/>
+        <v>86</v>
+      </c>
+      <c r="H6" s="67"/>
       <c r="I6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="56"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="64"/>
       <c r="E7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="54"/>
+        <v>95</v>
+      </c>
+      <c r="F7" s="56"/>
       <c r="G7" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" s="65"/>
+        <v>134</v>
+      </c>
+      <c r="H7" s="67"/>
       <c r="I7" s="7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="F8" s="56"/>
+      <c r="G8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="67"/>
+      <c r="I8" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="58"/>
+      <c r="C9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="64"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="67"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="58"/>
+      <c r="C10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="64"/>
+      <c r="E10" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="F10" s="56"/>
+      <c r="G10" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="67"/>
+      <c r="I10" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="58"/>
+      <c r="C11" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="F11" s="56"/>
+      <c r="G11" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="67"/>
+      <c r="I11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="58"/>
+      <c r="C12" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="D12" s="64"/>
+      <c r="E12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="56"/>
+      <c r="G12" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="67"/>
+      <c r="I12" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="58"/>
+      <c r="C13" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="D13" s="64"/>
+      <c r="E13" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="F13" s="56"/>
+      <c r="G13" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="67"/>
+      <c r="I13" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="58"/>
+      <c r="C14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="64"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="67"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="58"/>
+      <c r="C15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="64"/>
+      <c r="E15" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="F15" s="56"/>
+      <c r="G15" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="67"/>
+      <c r="I15" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="58"/>
+      <c r="C16" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" s="64"/>
+      <c r="E16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="6" t="s">
+      <c r="F16" s="56"/>
+      <c r="G16" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="67"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="58"/>
+      <c r="C17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="64"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H17" s="67"/>
+      <c r="I17" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="58"/>
+      <c r="C18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="64"/>
+      <c r="E18" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="F18" s="56"/>
+      <c r="G18" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H18" s="67"/>
+      <c r="I18" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="58"/>
+      <c r="C19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="64"/>
+      <c r="E19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="56"/>
+      <c r="G19" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="67"/>
+      <c r="I19" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="58"/>
+      <c r="C20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="64"/>
+      <c r="E20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="56"/>
+      <c r="G20" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="67"/>
+      <c r="I20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="58"/>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="64"/>
+      <c r="E21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="56"/>
+      <c r="G21" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="67"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="58"/>
+      <c r="C22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="64"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="67"/>
+      <c r="I22" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="58"/>
+      <c r="C23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="64"/>
+      <c r="E23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="56"/>
+      <c r="G23" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="67"/>
+      <c r="I23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="6" t="s">
+    </row>
+    <row r="24" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="58"/>
+      <c r="C24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="64"/>
+      <c r="E24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="56"/>
+      <c r="G24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="67"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="58"/>
+      <c r="C25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="64"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="67"/>
+      <c r="I25" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="58"/>
+      <c r="C26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="64"/>
+      <c r="E26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="56"/>
+      <c r="G26" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="67"/>
+      <c r="I26" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="58"/>
+      <c r="C27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="64"/>
+      <c r="E27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="56"/>
+      <c r="G27" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="67"/>
+      <c r="I27" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="58"/>
+      <c r="C28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="64"/>
+      <c r="E28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="56"/>
+      <c r="G28" s="10" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
-      <c r="C9" s="6" t="s">
+      <c r="H28" s="67"/>
+      <c r="I28" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="58"/>
+      <c r="C29" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="64"/>
+      <c r="E29" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="56"/>
+      <c r="G29" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="67"/>
+      <c r="I29" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="58"/>
+      <c r="C30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H9" s="65"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="56"/>
-      <c r="C10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="56"/>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="56"/>
-      <c r="C12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="54"/>
-      <c r="G12" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="56"/>
-      <c r="C13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="56"/>
-      <c r="C14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="62"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" s="65"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="56"/>
-      <c r="C15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="54"/>
-      <c r="G15" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="H15" s="65"/>
-      <c r="I15" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="56"/>
-      <c r="C16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="62"/>
-      <c r="E16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H16" s="65"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="56"/>
-      <c r="C17" s="6" t="s">
+      <c r="D30" s="64"/>
+      <c r="E30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="56"/>
+      <c r="G30" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="67"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="58"/>
+      <c r="C31" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="62"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="65"/>
-      <c r="I17" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="56"/>
-      <c r="C18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="62"/>
-      <c r="E18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H18" s="65"/>
-      <c r="I18" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="56"/>
-      <c r="C19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="62"/>
-      <c r="E19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H19" s="65"/>
-      <c r="I19" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="56"/>
-      <c r="C20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H20" s="65"/>
-      <c r="I20" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="56"/>
-      <c r="C21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="54"/>
-      <c r="G21" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="H21" s="65"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="56"/>
-      <c r="C22" s="6" t="s">
+      <c r="D31" s="64"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H31" s="67"/>
+      <c r="I31" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="58"/>
+      <c r="C32" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="6" t="s">
+      <c r="D32" s="64"/>
+      <c r="E32" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="56"/>
+      <c r="G32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H32" s="67"/>
+      <c r="I32" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="58"/>
+      <c r="C33" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="64"/>
+      <c r="E33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="56"/>
+      <c r="G33" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="67"/>
+      <c r="I33" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="58"/>
+      <c r="C34" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="64"/>
+      <c r="E34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="56"/>
+      <c r="G34" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="67"/>
+      <c r="I34" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="58"/>
+      <c r="C35" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="64"/>
+      <c r="E35" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="56"/>
+      <c r="G35" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="H35" s="67"/>
+      <c r="I35" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="58"/>
+      <c r="C36" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D36" s="64"/>
+      <c r="E36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="56"/>
+      <c r="G36" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H36" s="67"/>
+      <c r="I36" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="58"/>
+      <c r="C37" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D37" s="64"/>
+      <c r="E37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="56"/>
+      <c r="G37" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H37" s="67"/>
+      <c r="I37" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="58"/>
+      <c r="C38" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" s="64"/>
+      <c r="E38" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="56"/>
+      <c r="G38" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H38" s="67"/>
+      <c r="I38" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="58"/>
+      <c r="C39" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D39" s="64"/>
+      <c r="E39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="56"/>
+      <c r="G39" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H39" s="67"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="58"/>
+      <c r="C40" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D40" s="64"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H22" s="65"/>
-      <c r="I22" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="56"/>
-      <c r="C23" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="54"/>
-      <c r="G23" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H23" s="65"/>
-      <c r="I23" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="56"/>
-      <c r="C24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="54"/>
-      <c r="G24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="65"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="56"/>
-      <c r="C25" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="65"/>
-      <c r="I25" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="56"/>
-      <c r="C26" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="54"/>
-      <c r="G26" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" s="65"/>
-      <c r="I26" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="56"/>
-      <c r="C27" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="54"/>
-      <c r="G27" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" s="65"/>
-      <c r="I27" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="56"/>
-      <c r="C28" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="54"/>
-      <c r="G28" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="65"/>
-      <c r="I28" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="56"/>
-      <c r="C29" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" s="54"/>
-      <c r="G29" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="H29" s="65"/>
-      <c r="I29" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="56"/>
-      <c r="C30" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="62"/>
-      <c r="E30" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="54"/>
-      <c r="G30" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H30" s="65"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="56"/>
-      <c r="C31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="62"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H31" s="65"/>
-      <c r="I31" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="56"/>
-      <c r="C32" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="54"/>
-      <c r="G32" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H32" s="65"/>
-      <c r="I32" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="56"/>
-      <c r="C33" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="62"/>
-      <c r="E33" s="6" t="s">
+      <c r="H40" s="67"/>
+      <c r="I40" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="58"/>
+      <c r="C41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="64"/>
+      <c r="E41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="54"/>
-      <c r="G33" s="10" t="s">
+      <c r="F41" s="56"/>
+      <c r="G41" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H41" s="67"/>
+      <c r="I41" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H33" s="65"/>
-      <c r="I33" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="56"/>
-      <c r="C34" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="62"/>
-      <c r="E34" s="6" t="s">
+    </row>
+    <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="58"/>
+      <c r="C42" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="64"/>
+      <c r="E42" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="F42" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="I42" s="60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="58"/>
+      <c r="C43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="64"/>
+      <c r="E43" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="F43" s="56"/>
+      <c r="G43" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="56"/>
+      <c r="I43" s="61"/>
+    </row>
+    <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="51"/>
+      <c r="C44" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="65"/>
+      <c r="E44" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="54"/>
-      <c r="G34" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H34" s="65"/>
-      <c r="I34" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="56"/>
-      <c r="C35" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" s="62"/>
-      <c r="E35" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="54"/>
-      <c r="G35" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="H35" s="65"/>
-      <c r="I35" s="7" t="s">
+      <c r="F44" s="57"/>
+      <c r="G44" s="15" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="56"/>
-      <c r="C36" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="D36" s="62"/>
-      <c r="E36" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="54"/>
-      <c r="G36" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="H36" s="65"/>
-      <c r="I36" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="56"/>
-      <c r="C37" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="D37" s="62"/>
-      <c r="E37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="54"/>
-      <c r="G37" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="H37" s="65"/>
-      <c r="I37" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="56"/>
-      <c r="C38" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="D38" s="62"/>
-      <c r="E38" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" s="54"/>
-      <c r="G38" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="H38" s="65"/>
-      <c r="I38" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="56"/>
-      <c r="C39" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="D39" s="62"/>
-      <c r="E39" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F39" s="54"/>
-      <c r="G39" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="H39" s="65"/>
-      <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="56"/>
-      <c r="C40" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="D40" s="62"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H40" s="65"/>
-      <c r="I40" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="56"/>
-      <c r="C41" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="62"/>
-      <c r="E41" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="54"/>
-      <c r="G41" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H41" s="65"/>
-      <c r="I41" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="56"/>
-      <c r="C42" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="62"/>
-      <c r="E42" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H42" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="I42" s="58" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="56"/>
-      <c r="C43" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="62"/>
-      <c r="E43" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H43" s="54"/>
-      <c r="I43" s="59"/>
-    </row>
-    <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="49"/>
-      <c r="C44" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="63"/>
-      <c r="E44" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="55"/>
-      <c r="G44" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="H44" s="55"/>
-      <c r="I44" s="60"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="62"/>
     </row>
     <row r="45" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
@@ -4754,8 +4901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4775,89 +4922,89 @@
     <row r="1" spans="2:9" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="35" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="30" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="33" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I3" s="38"/>
     </row>
     <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G4" s="28"/>
       <c r="H4" s="24" t="s">
-        <v>371</v>
+        <v>421</v>
       </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="24"/>
@@ -4865,19 +5012,19 @@
     </row>
     <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="24"/>
@@ -4885,19 +5032,19 @@
     </row>
     <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="24"/>
@@ -4905,19 +5052,19 @@
     </row>
     <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="24"/>
@@ -4925,92 +5072,92 @@
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="24" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="41" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="F10" s="46" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="G10" s="46"/>
       <c r="H10" s="45" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="I10" s="47"/>
     </row>
     <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="20" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="24" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="G12" s="28"/>
       <c r="H12" s="24"/>
       <c r="I12" s="7" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -5025,41 +5172,41 @@
     </row>
     <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>397</v>
+        <v>424</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>398</v>
+        <v>425</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="24" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="20" t="s">
-        <v>174</v>
+        <v>426</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>238</v>
+        <v>427</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>236</v>
+        <v>428</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="23"/>
@@ -5067,517 +5214,517 @@
     </row>
     <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="23" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="20" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="23" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="20" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="20" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>29</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>306</v>
+        <v>438</v>
       </c>
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="20" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>28</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="20" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="20" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="20" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="20" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="E27" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="23" t="s">
         <v>326</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>338</v>
       </c>
       <c r="I27" s="7"/>
     </row>
     <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="20" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="20" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="E29" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="23" t="s">
         <v>328</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="23" t="s">
-        <v>340</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="20" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C30" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="D30" s="24" t="s">
-        <v>331</v>
-      </c>
       <c r="E30" s="24" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="20" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G32" s="28"/>
       <c r="H32" s="23" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="20" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G33" s="28"/>
       <c r="H33" s="23"/>
       <c r="I33" s="7" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="20" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="23" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="20" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="23"/>
       <c r="I35" s="7" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="20" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="23" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="20" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="23"/>
@@ -5585,236 +5732,236 @@
     </row>
     <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="20" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="23" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="20" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="24" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B40" s="20" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="24" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="41" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D41" s="45" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E41" s="45" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="F41" s="46" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G41" s="46"/>
       <c r="H41" s="45" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="I41" s="47" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="20" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="24" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="41" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D43" s="45" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E43" s="45" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="F43" s="46" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G43" s="46"/>
       <c r="H43" s="45" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="I43" s="47" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="20" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="24" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="40" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G45" s="28"/>
       <c r="H45" s="24" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="40" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="G46" s="28"/>
       <c r="H46" s="23" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="20" t="s">
-        <v>372</v>
+        <v>420</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>373</v>
+        <v>422</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>374</v>
+        <v>423</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="G47" s="28"/>
       <c r="H47" s="23" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6331,79 +6478,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.125" style="66" customWidth="1"/>
-    <col min="4" max="4" width="32" style="66" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="66" customWidth="1"/>
-    <col min="6" max="6" width="32" style="66" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="32" style="48" customWidth="1"/>
+    <col min="5" max="5" width="15.125" style="48" customWidth="1"/>
+    <col min="6" max="6" width="32" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="66" t="s">
-        <v>422</v>
-      </c>
-      <c r="D13" s="66">
+      <c r="C13" s="48" t="s">
+        <v>404</v>
+      </c>
+      <c r="D13" s="48">
         <v>1</v>
       </c>
-      <c r="E13" s="66" t="s">
-        <v>429</v>
-      </c>
-      <c r="F13" s="66" t="s">
-        <v>434</v>
+      <c r="E13" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="66" t="s">
-        <v>423</v>
-      </c>
-      <c r="D14" s="66" t="s">
-        <v>432</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>427</v>
-      </c>
-      <c r="F14" s="66" t="s">
-        <v>435</v>
+      <c r="C14" s="48" t="s">
+        <v>405</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>414</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="66" t="s">
-        <v>424</v>
-      </c>
-      <c r="D15" s="66" t="s">
-        <v>433</v>
-      </c>
-      <c r="E15" s="66" t="s">
-        <v>428</v>
-      </c>
-      <c r="F15" s="66" t="s">
-        <v>436</v>
+      <c r="C15" s="48" t="s">
+        <v>406</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>415</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>410</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="66" t="s">
-        <v>425</v>
-      </c>
-      <c r="D16" s="67">
+      <c r="C16" s="48" t="s">
+        <v>407</v>
+      </c>
+      <c r="D16" s="49">
         <v>44280</v>
       </c>
-      <c r="E16" s="66" t="s">
-        <v>430</v>
-      </c>
-      <c r="F16" s="66" t="s">
-        <v>437</v>
+      <c r="E16" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="66" t="s">
-        <v>426</v>
-      </c>
-      <c r="D17" s="67">
+      <c r="C17" s="48" t="s">
+        <v>408</v>
+      </c>
+      <c r="D17" s="49">
         <v>44297</v>
       </c>
-      <c r="E17" s="66" t="s">
-        <v>431</v>
-      </c>
-      <c r="F17" s="67">
+      <c r="E17" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="F17" s="49">
         <v>44286</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0406 on_jQuery Error Commit
</commit_message>
<xml_diff>
--- a/프로젝트 기획서_콜미백.xlsx
+++ b/프로젝트 기획서_콜미백.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17685"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="447">
   <si>
     <t>프로젝트 기획서</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2618,6 +2618,10 @@
   </si>
   <si>
     <t>(마우스오버) 팜플렛, 책자 등 일반 인쇄용 고화질 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jQuery -3.6.0.min.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3575,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D22:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3791,6 +3795,9 @@
     </row>
     <row r="27" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
+      <c r="C27" s="3" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="28" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
@@ -3875,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4901,8 +4908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
0407 ViewPages Finished Commit
</commit_message>
<xml_diff>
--- a/프로젝트 기획서_콜미백.xlsx
+++ b/프로젝트 기획서_콜미백.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="개요" sheetId="1" r:id="rId1"/>
@@ -3043,7 +3043,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3247,6 +3247,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3579,7 +3582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3882,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4908,8 +4911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5671,25 +5674,25 @@
         <v>290</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="20" t="s">
+    <row r="35" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="43" t="s">
         <v>353</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="45" t="s">
         <v>354</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="7" t="s">
+      <c r="G35" s="46"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="47" t="s">
         <v>341</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0408 DB Build Commit
</commit_message>
<xml_diff>
--- a/프로젝트 기획서_콜미백.xlsx
+++ b/프로젝트 기획서_콜미백.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="450">
   <si>
     <t>프로젝트 기획서</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -209,34 +209,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>프로젝트(프로젝트명,프로젝트ID,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>의뢰인 ID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,구분s,등록일자,관리자확인일자,프로젝트 구분) - 구분s : 하단 프로젝트 구분 참고</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사진 - 인물 - 화보 - 의류 및 잡화 - 의류</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2238,10 +2210,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원(이름, 아이디, 비밀번호, 가입일자, 생성 프로젝트 갯수)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>profile.jsp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2622,6 +2590,26 @@
   </si>
   <si>
     <t>jQuery -3.6.0.min.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트(회원/비회원구분, 프로젝트명,프로젝트ID, PW, 등록인 ID, 구분s,등록일자, 마감일, 셀프/의뢰 구분, 상세설명, 제작자ID, 레퍼런스 파일 갯수) - 구분s :  구분탭 참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원(이름, 아이디, 비밀번호, 가입일자)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(누끼)basic, (컨셉)productConcept, (착용)productWear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(조리)cooking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basicWear, detailWear, etc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2629,7 +2617,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2699,14 +2687,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="4"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -3043,7 +3023,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3194,6 +3174,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3247,9 +3233,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3583,7 +3566,7 @@
   <dimension ref="B1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3598,12 +3581,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
     </row>
     <row r="3" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -3648,37 +3631,37 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="53"/>
+      <c r="C7" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="50" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="51"/>
-      <c r="C7" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="12" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="8" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="57" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="52" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="13" t="s">
@@ -3686,55 +3669,55 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="58"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="56"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="51" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="56"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" s="56"/>
+        <v>151</v>
+      </c>
+      <c r="D11" s="58"/>
       <c r="E11" s="6" t="s">
-        <v>390</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="56"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="56"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="6" t="s">
-        <v>32</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="57"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="57"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3742,21 +3725,21 @@
     </row>
     <row r="15" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3784,7 +3767,7 @@
     <row r="24" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3793,13 +3776,13 @@
     <row r="26" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3885,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42:I44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3905,758 +3888,758 @@
   <sheetData>
     <row r="1" spans="2:9" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
-        <v>83</v>
+      <c r="B2" s="52" t="s">
+        <v>82</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="63" t="s">
-        <v>443</v>
+      <c r="D2" s="65" t="s">
+        <v>441</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>151</v>
+        <v>36</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>150</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" s="66" t="s">
-        <v>150</v>
+        <v>122</v>
+      </c>
+      <c r="H2" s="68" t="s">
+        <v>149</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="F3" s="56"/>
+        <v>427</v>
+      </c>
+      <c r="F3" s="58"/>
       <c r="G3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="67"/>
+        <v>83</v>
+      </c>
+      <c r="H3" s="69"/>
       <c r="I3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="58"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="64"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="56"/>
+        <v>43</v>
+      </c>
+      <c r="F4" s="58"/>
       <c r="G4" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="67"/>
+        <v>84</v>
+      </c>
+      <c r="H4" s="69"/>
       <c r="I4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="58"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="F5" s="58"/>
+      <c r="G5" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H5" s="69"/>
+      <c r="I5" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="6" t="s">
-        <v>430</v>
-      </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="H5" s="67"/>
-      <c r="I5" s="6" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="58"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="64"/>
+      <c r="D6" s="66"/>
       <c r="E6" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="F6" s="56"/>
+        <v>429</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" s="67"/>
+        <v>85</v>
+      </c>
+      <c r="H6" s="69"/>
       <c r="I6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="58"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="64"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="56"/>
+        <v>94</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="69"/>
+      <c r="I7" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="67"/>
-      <c r="I7" s="7" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="64"/>
+      <c r="D8" s="66"/>
       <c r="E8" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="69"/>
+      <c r="I8" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="60"/>
+      <c r="C9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="66"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="69"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="60"/>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="69"/>
+      <c r="I10" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="60"/>
+      <c r="C11" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="67"/>
-      <c r="I8" s="6" t="s">
+      <c r="F11" s="58"/>
+      <c r="G11" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="69"/>
+      <c r="I11" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60"/>
+      <c r="C12" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="58"/>
+      <c r="G12" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="69"/>
+      <c r="I12" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="60"/>
+      <c r="C13" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="D13" s="66"/>
+      <c r="E13" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="69"/>
+      <c r="I13" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="60"/>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="66"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="69"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="60"/>
+      <c r="C15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="66"/>
+      <c r="E15" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="F15" s="58"/>
+      <c r="G15" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" s="69"/>
+      <c r="I15" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="60"/>
+      <c r="C16" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="D16" s="66"/>
+      <c r="E16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="69"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="60"/>
+      <c r="C17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="66"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H17" s="69"/>
+      <c r="I17" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="60"/>
+      <c r="C18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="66"/>
+      <c r="E18" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="F18" s="58"/>
+      <c r="G18" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="69"/>
+      <c r="I18" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="60"/>
+      <c r="C19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="66"/>
+      <c r="E19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="69"/>
+      <c r="I19" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="60"/>
+      <c r="C20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="66"/>
+      <c r="E20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="58"/>
+      <c r="G20" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" s="69"/>
+      <c r="I20" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="60"/>
+      <c r="C21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="66"/>
+      <c r="E21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="58"/>
+      <c r="G21" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" s="69"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="60"/>
+      <c r="C22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="66"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="69"/>
+      <c r="I22" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="60"/>
+      <c r="C23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="66"/>
+      <c r="E23" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
-      <c r="C9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="6" t="s">
+      <c r="F23" s="58"/>
+      <c r="G23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
-      <c r="C10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="H10" s="67"/>
-      <c r="I10" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
-      <c r="C11" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="H11" s="67"/>
-      <c r="I11" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
-      <c r="C12" s="6" t="s">
-        <v>435</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="56"/>
-      <c r="G12" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H12" s="67"/>
-      <c r="I12" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
-      <c r="C13" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="F13" s="56"/>
-      <c r="G13" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="H13" s="67"/>
-      <c r="I13" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
-      <c r="C14" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="67"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
-      <c r="C15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="F15" s="56"/>
-      <c r="G15" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H15" s="67"/>
-      <c r="I15" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
-      <c r="C16" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H16" s="67"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
-      <c r="C17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H17" s="67"/>
-      <c r="I17" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
-      <c r="C18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18" s="67"/>
-      <c r="I18" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58"/>
-      <c r="C19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="67"/>
-      <c r="I19" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="58"/>
-      <c r="C20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H20" s="67"/>
-      <c r="I20" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="58"/>
-      <c r="C21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H21" s="67"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="58"/>
-      <c r="C22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H22" s="67"/>
-      <c r="I22" s="7" t="s">
+      <c r="H23" s="69"/>
+      <c r="I23" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="58"/>
-      <c r="C23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="67"/>
-      <c r="I23" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
     <row r="24" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="58"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="64"/>
+      <c r="D24" s="66"/>
       <c r="E24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="56"/>
+        <v>52</v>
+      </c>
+      <c r="F24" s="58"/>
       <c r="G24" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="67"/>
+        <v>93</v>
+      </c>
+      <c r="H24" s="69"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="58"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="66"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="69"/>
+      <c r="I25" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="60"/>
+      <c r="C26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="66"/>
+      <c r="E26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="58"/>
+      <c r="G26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="69"/>
+      <c r="I26" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="60"/>
+      <c r="C27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="66"/>
+      <c r="E27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="G27" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="69"/>
+      <c r="I27" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="60"/>
+      <c r="C28" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="66"/>
+      <c r="E28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="G28" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="69"/>
+      <c r="I28" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="60"/>
+      <c r="C29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="66"/>
+      <c r="E29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H29" s="69"/>
+      <c r="I29" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="60"/>
+      <c r="C30" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H25" s="67"/>
-      <c r="I25" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="58"/>
-      <c r="C26" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="7" t="s">
+      <c r="D30" s="66"/>
+      <c r="E30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="58"/>
+      <c r="G30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="69"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="60"/>
+      <c r="C31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="66"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="69"/>
+      <c r="I31" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="60"/>
+      <c r="C32" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="66"/>
+      <c r="E32" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="58"/>
+      <c r="G32" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="69"/>
+      <c r="I32" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="60"/>
+      <c r="C33" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="66"/>
+      <c r="E33" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="58"/>
+      <c r="G33" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="69"/>
+      <c r="I33" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="60"/>
+      <c r="C34" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="66"/>
+      <c r="E34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="58"/>
+      <c r="G34" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="69"/>
+      <c r="I34" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="60"/>
+      <c r="C35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="66"/>
+      <c r="E35" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="58"/>
+      <c r="G35" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="H35" s="69"/>
+      <c r="I35" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="60"/>
+      <c r="C36" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D36" s="66"/>
+      <c r="E36" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="56"/>
-      <c r="G26" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H26" s="67"/>
-      <c r="I26" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="58"/>
-      <c r="C27" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H27" s="67"/>
-      <c r="I27" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="58"/>
-      <c r="C28" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="56"/>
-      <c r="G28" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H28" s="67"/>
-      <c r="I28" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="58"/>
-      <c r="C29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="56"/>
-      <c r="G29" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="67"/>
-      <c r="I29" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="58"/>
-      <c r="C30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" s="56"/>
-      <c r="G30" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H30" s="67"/>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="58"/>
-      <c r="C31" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H31" s="67"/>
-      <c r="I31" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="58"/>
-      <c r="C32" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="56"/>
-      <c r="G32" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H32" s="67"/>
-      <c r="I32" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="58"/>
-      <c r="C33" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="56"/>
-      <c r="G33" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H33" s="67"/>
-      <c r="I33" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="58"/>
-      <c r="C34" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="6" t="s">
+      <c r="F36" s="58"/>
+      <c r="G36" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="H36" s="69"/>
+      <c r="I36" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="56"/>
-      <c r="G34" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H34" s="67"/>
-      <c r="I34" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="58"/>
-      <c r="C35" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="H35" s="67"/>
-      <c r="I35" s="7" t="s">
+    </row>
+    <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="60"/>
+      <c r="C37" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D37" s="66"/>
+      <c r="E37" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="58"/>
+      <c r="G37" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H37" s="69"/>
+      <c r="I37" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="60"/>
+      <c r="C38" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D38" s="66"/>
+      <c r="E38" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="58"/>
+      <c r="G38" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H38" s="69"/>
+      <c r="I38" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="60"/>
+      <c r="C39" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="66"/>
+      <c r="E39" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="58"/>
+      <c r="G39" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H39" s="69"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="60"/>
+      <c r="C40" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D40" s="66"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="58"/>
-      <c r="C36" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="H36" s="67"/>
-      <c r="I36" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="58"/>
-      <c r="C37" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" s="56"/>
-      <c r="G37" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="H37" s="67"/>
-      <c r="I37" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="58"/>
-      <c r="C38" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="56"/>
-      <c r="G38" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="H38" s="67"/>
-      <c r="I38" s="6" t="s">
+      <c r="H40" s="69"/>
+      <c r="I40" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="60"/>
+      <c r="C41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="66"/>
+      <c r="E41" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="58"/>
-      <c r="C39" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="56"/>
-      <c r="G39" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="H39" s="67"/>
-      <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="58"/>
-      <c r="C40" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="H40" s="67"/>
-      <c r="I40" s="6" t="s">
+      <c r="F41" s="58"/>
+      <c r="G41" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="58"/>
-      <c r="C41" s="6" t="s">
+      <c r="H41" s="69"/>
+      <c r="I41" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="60"/>
+      <c r="C42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="64"/>
-      <c r="E41" s="7" t="s">
+      <c r="D42" s="66"/>
+      <c r="E42" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="F42" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="I42" s="62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="60"/>
+      <c r="C43" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="66"/>
+      <c r="E43" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="F43" s="58"/>
+      <c r="G43" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="58"/>
+      <c r="I43" s="63"/>
+    </row>
+    <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="53"/>
+      <c r="C44" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" s="67"/>
+      <c r="E44" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="56"/>
-      <c r="G41" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H41" s="67"/>
-      <c r="I41" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="58"/>
-      <c r="C42" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="F42" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H42" s="55" t="s">
+      <c r="F44" s="59"/>
+      <c r="G44" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I42" s="60" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="58"/>
-      <c r="C43" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="64"/>
-      <c r="E43" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="F43" s="56"/>
-      <c r="G43" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H43" s="56"/>
-      <c r="I43" s="61"/>
-    </row>
-    <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="51"/>
-      <c r="C44" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="65"/>
-      <c r="E44" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F44" s="57"/>
-      <c r="G44" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="H44" s="57"/>
-      <c r="I44" s="62"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="64"/>
     </row>
     <row r="45" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
@@ -4911,8 +4894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4932,89 +4915,89 @@
     <row r="1" spans="2:9" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I3" s="38"/>
     </row>
     <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G4" s="28"/>
       <c r="H4" s="24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>184</v>
-      </c>
       <c r="F5" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="24"/>
@@ -5022,19 +5005,19 @@
     </row>
     <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>188</v>
-      </c>
       <c r="E6" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="24"/>
@@ -5042,19 +5025,19 @@
     </row>
     <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>186</v>
-      </c>
       <c r="E7" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="24"/>
@@ -5062,19 +5045,19 @@
     </row>
     <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>384</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="D8" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>386</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="28" t="s">
         <v>387</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>388</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="24"/>
@@ -5082,92 +5065,92 @@
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C9" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="28" t="s">
         <v>369</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>370</v>
       </c>
       <c r="G9" s="28"/>
       <c r="H9" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>378</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="D10" s="44" t="s">
         <v>372</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="E10" s="45" t="s">
         <v>373</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="F10" s="46" t="s">
         <v>374</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>375</v>
       </c>
       <c r="G10" s="46"/>
       <c r="H10" s="45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I10" s="47"/>
     </row>
     <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="E11" s="24" t="s">
         <v>393</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="F11" s="28" t="s">
         <v>394</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>395</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>396</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>397</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D12" s="25" t="s">
+      <c r="E12" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>399</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>389</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>401</v>
       </c>
       <c r="G12" s="28"/>
       <c r="H12" s="24"/>
       <c r="I12" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -5182,41 +5165,41 @@
     </row>
     <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>423</v>
+      </c>
+      <c r="E14" s="24" t="s">
         <v>380</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="E14" s="24" t="s">
+      <c r="F14" s="28" t="s">
         <v>381</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>382</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>426</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>427</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>428</v>
-      </c>
       <c r="E15" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="23"/>
@@ -5224,517 +5207,521 @@
     </row>
     <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="D16" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="E16" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="F16" s="28" t="s">
         <v>230</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>231</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="D17" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="E17" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>235</v>
-      </c>
       <c r="F17" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="D18" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="D18" s="24" t="s">
-        <v>245</v>
-      </c>
       <c r="E18" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="D19" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>248</v>
-      </c>
       <c r="E19" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E20" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>253</v>
-      </c>
       <c r="H20" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="D22" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="E22" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>270</v>
-      </c>
       <c r="F22" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G22" s="24" t="s">
         <v>29</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="D23" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="E23" s="24" t="s">
         <v>273</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>274</v>
-      </c>
       <c r="F23" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>28</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>326</v>
+        <v>449</v>
       </c>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="D24" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="E24" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>278</v>
-      </c>
       <c r="F24" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G26" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="I27" s="7"/>
+        <v>325</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C29" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>320</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>316</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>306</v>
-      </c>
       <c r="G29" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H29" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="D31" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="E31" s="24" t="s">
         <v>310</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>311</v>
-      </c>
       <c r="F31" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>328</v>
-      </c>
-      <c r="I31" s="7"/>
+        <v>327</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="D32" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="E32" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>324</v>
-      </c>
       <c r="F32" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G32" s="28"/>
       <c r="H32" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="D33" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="E33" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="E33" s="24" t="s">
-        <v>282</v>
-      </c>
       <c r="F33" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G33" s="28"/>
       <c r="H33" s="23"/>
       <c r="I33" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="D34" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="E34" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="F34" s="28" t="s">
         <v>288</v>
-      </c>
-      <c r="F34" s="28" t="s">
-        <v>289</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="41" t="s">
+        <v>351</v>
+      </c>
+      <c r="C35" s="43" t="s">
         <v>352</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="D35" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="D35" s="45" t="s">
-        <v>354</v>
-      </c>
       <c r="E35" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F35" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G35" s="46"/>
-      <c r="H35" s="68"/>
+      <c r="H35" s="50"/>
       <c r="I35" s="47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D36" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="E36" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="F36" s="28" t="s">
         <v>339</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>340</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="23"/>
@@ -5742,236 +5729,236 @@
     </row>
     <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="D38" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>329</v>
-      </c>
-      <c r="D38" s="24" t="s">
+      <c r="E38" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="F38" s="28" t="s">
         <v>332</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>333</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>167</v>
-      </c>
       <c r="E39" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B40" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="D40" s="24" t="s">
-        <v>175</v>
-      </c>
       <c r="E40" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="C41" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" s="45" t="s">
+      <c r="E41" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="E41" s="45" t="s">
-        <v>193</v>
-      </c>
       <c r="F41" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G41" s="46"/>
       <c r="H41" s="45" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I41" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="D42" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="D42" s="24" t="s">
+      <c r="E42" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="E42" s="24" t="s">
-        <v>220</v>
-      </c>
       <c r="F42" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="2:9" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C43" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="D43" s="45" t="s">
-        <v>195</v>
-      </c>
       <c r="E43" s="45" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F43" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G43" s="46"/>
       <c r="H43" s="45" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I43" s="47" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="D44" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="D44" s="24" t="s">
-        <v>347</v>
-      </c>
       <c r="E44" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G44" s="28"/>
       <c r="H44" s="24" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>173</v>
-      </c>
       <c r="E45" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G45" s="28"/>
       <c r="H45" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="D46" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="E46" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="F46" s="28" t="s">
         <v>224</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>225</v>
       </c>
       <c r="G46" s="28"/>
       <c r="H46" s="23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="C47" s="22" t="s">
         <v>420</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>422</v>
-      </c>
       <c r="D47" s="24" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E47" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="F47" s="28" t="s">
         <v>359</v>
-      </c>
-      <c r="F47" s="28" t="s">
-        <v>360</v>
       </c>
       <c r="G47" s="28"/>
       <c r="H47" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="I47" s="7" t="s">
         <v>361</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6496,69 +6483,69 @@
   <sheetData>
     <row r="13" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C13" s="48" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D13" s="48">
         <v>1</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C14" s="48" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C15" s="48" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F15" s="48" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C16" s="48" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D16" s="49">
         <v>44280</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="48" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D17" s="49">
         <v>44297</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F17" s="49">
         <v>44286</v>

</xml_diff>